<commit_message>
Day 5 Fourth Commit Implemented PlaceMedicineOrder flow: Added steps to fill patient form, click save and confirm, and proceed to payments tab. Includes proper waits to ensure buttons are clickable and page navigation works smoothly.
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/InputData.xlsx
+++ b/src/test/resources/Exceldata/InputData.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0124D322-8EA0-4FD1-B67C-9089A37D579A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -51,8 +53,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,9 +105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +145,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -177,6 +179,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -211,9 +214,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,14 +390,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.1796875" customWidth="1"/>
@@ -401,7 +405,7 @@
     <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,12 +425,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>8778922710</v>
+        <v>6379948639</v>
       </c>
       <c r="B2">
-        <v>600096</v>
+        <v>600003</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -441,7 +445,7 @@
         <v>38139</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -452,24 +456,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>